<commit_message>
change name from flex
</commit_message>
<xml_diff>
--- a/WRX_SAP INTERFACE/Flex_Data_structure.xlsx
+++ b/WRX_SAP INTERFACE/Flex_Data_structure.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\flex\WRX_SAP INTERFACE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D30B15A3-14CE-41AD-A92A-BCCE4FBB1712}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B97530B5-CE97-4CBF-A56B-E0FA8C3162EA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{12C5C8EF-92D1-47ED-8473-DFC0E0C05236}"/>
+    <workbookView xWindow="1395" yWindow="2355" windowWidth="21600" windowHeight="11385" xr2:uid="{12C5C8EF-92D1-47ED-8473-DFC0E0C05236}"/>
   </bookViews>
   <sheets>
     <sheet name="Menu" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="310">
   <si>
     <t>Menu Group</t>
   </si>
@@ -955,6 +955,18 @@
   </si>
   <si>
     <t>consign_check, consign_check_detail</t>
+  </si>
+  <si>
+    <t>DBSALE</t>
+  </si>
+  <si>
+    <t>พนักงานขาย</t>
+  </si>
+  <si>
+    <t>Sale_man</t>
+  </si>
+  <si>
+    <t>saleman</t>
   </si>
 </sst>
 </file>
@@ -10349,8 +10361,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB82F9EC-2777-44E0-A7BB-7F93552DDD25}">
   <dimension ref="B3:P77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="K76" sqref="K76"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10831,22 +10843,22 @@
       </c>
     </row>
     <row r="24" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="F24" s="3" t="s">
+      <c r="F24" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="G24" s="3" t="s">
+      <c r="G24" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="H24" s="4" t="s">
+      <c r="H24" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I24" s="3" t="s">
+      <c r="I24" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="J24" s="3" t="s">
+      <c r="J24" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="K24" s="3" t="s">
+      <c r="K24" s="5" t="s">
         <v>265</v>
       </c>
     </row>
@@ -10891,12 +10903,24 @@
       </c>
     </row>
     <row r="27" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
-      <c r="K27" s="3"/>
+      <c r="F27" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="J27" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="K27" s="3" t="s">
+        <v>309</v>
+      </c>
     </row>
     <row r="28" spans="5:11" x14ac:dyDescent="0.25">
       <c r="F28" s="3" t="s">
@@ -11232,22 +11256,22 @@
       </c>
     </row>
     <row r="43" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="F43" s="3" t="s">
+      <c r="F43" s="5" t="s">
         <v>288</v>
       </c>
-      <c r="G43" s="3" t="s">
+      <c r="G43" s="5" t="s">
         <v>283</v>
       </c>
-      <c r="H43" s="4" t="s">
+      <c r="H43" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="I43" s="3" t="s">
+      <c r="I43" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="J43" s="3" t="s">
+      <c r="J43" s="5" t="s">
         <v>304</v>
       </c>
-      <c r="K43" s="3" t="s">
+      <c r="K43" s="5" t="s">
         <v>305</v>
       </c>
     </row>
@@ -11588,22 +11612,22 @@
     </row>
     <row r="66" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E66" s="34"/>
-      <c r="F66" s="3" t="s">
+      <c r="F66" s="5" t="s">
         <v>300</v>
       </c>
-      <c r="G66" s="3" t="s">
+      <c r="G66" s="5" t="s">
         <v>284</v>
       </c>
-      <c r="H66" s="4" t="s">
+      <c r="H66" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="I66" s="3" t="s">
+      <c r="I66" s="5" t="s">
         <v>301</v>
       </c>
-      <c r="J66" s="3" t="s">
+      <c r="J66" s="5" t="s">
         <v>302</v>
       </c>
-      <c r="K66" s="3" t="s">
+      <c r="K66" s="5" t="s">
         <v>303</v>
       </c>
     </row>

</xml_diff>